<commit_message>
Update description et fix compilation 4c748b5c1934d12077dd9f4349504a80b6ddf02c
</commit_message>
<xml_diff>
--- a/299-Ajout-de-l'évaluation/ig/CodeSystem-input-tddui-task-transport-codesystem.xlsx
+++ b/299-Ajout-de-l'évaluation/ig/CodeSystem-input-tddui-task-transport-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-ballot</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-15T15:04:22+00:00</t>
+    <t>2025-10-16T14:47:34+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -186,7 +186,7 @@
     <t>accompagnement</t>
   </si>
   <si>
-    <t>Accompagnement nécessaire ou non de l'usager.</t>
+    <t xml:space="preserve">Accompagnement nécessaire ou non de l'usager. </t>
   </si>
   <si>
     <t>asepsie</t>

</xml_diff>